<commit_message>
This is the third commit
</commit_message>
<xml_diff>
--- a/src/TestData/IHTSOA.xlsx
+++ b/src/TestData/IHTSOA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14505" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>TestSuit</t>
   </si>
@@ -396,7 +396,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -434,9 +434,6 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:4" customFormat="1">
       <c r="A4" t="s">
@@ -445,9 +442,6 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="5" spans="1:4" customFormat="1">
       <c r="A5" t="s">
@@ -456,9 +450,6 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
@@ -467,9 +458,6 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
@@ -510,9 +498,6 @@
       </c>
       <c r="B10" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
This is 5th commit
</commit_message>
<xml_diff>
--- a/src/TestData/IHTSOA.xlsx
+++ b/src/TestData/IHTSOA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13470" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>TestSuit</t>
   </si>
@@ -37,39 +37,68 @@
     <t>GetSpeeds</t>
   </si>
   <si>
+    <t>OamTest_new</t>
+  </si>
+  <si>
+    <t>OpenCloseService</t>
+  </si>
+  <si>
+    <t>CreateCrossConnetc</t>
+  </si>
+  <si>
+    <t>DeleteCrossConnetc</t>
+  </si>
+  <si>
+    <t>Get_tech_profile_list</t>
+  </si>
+  <si>
+    <t>CreateRouterConfig</t>
+  </si>
+  <si>
+    <t>GetAccesspoint</t>
+  </si>
+  <si>
+    <t>TG300006</t>
+  </si>
+  <si>
+    <t>channel_id</t>
+  </si>
+  <si>
+    <t>dslam</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>sik</t>
+  </si>
+  <si>
+    <t>PS300206</t>
+  </si>
+  <si>
+    <t>apt4xda5</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
     <t>Retrain</t>
-  </si>
-  <si>
-    <t>OamTest_new</t>
-  </si>
-  <si>
-    <t>OpenCloseService</t>
-  </si>
-  <si>
-    <t>CreateCrossConnetc</t>
-  </si>
-  <si>
-    <t>DeleteCrossConnetc</t>
-  </si>
-  <si>
-    <t>Get_tech_profile_list</t>
-  </si>
-  <si>
-    <t>CreateRouterConfig</t>
-  </si>
-  <si>
-    <t>GetAccesspoint</t>
-  </si>
-  <si>
-    <t>TG300006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -93,12 +122,162 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,126 +572,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" customFormat="1">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" customFormat="1">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
This is 6th commit
</commit_message>
<xml_diff>
--- a/src/TestData/IHTSOA.xlsx
+++ b/src/TestData/IHTSOA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13470" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13365" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>TestSuit</t>
   </si>
@@ -79,10 +79,31 @@
     <t>apt4xda5</t>
   </si>
   <si>
-    <t>1s</t>
-  </si>
-  <si>
     <t>Retrain</t>
+  </si>
+  <si>
+    <t>PS200207</t>
+  </si>
+  <si>
+    <t>aptxdd1</t>
+  </si>
+  <si>
+    <t>test_speed</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>technical_profile_name</t>
+  </si>
+  <si>
+    <t>F40000/70000-T</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>PS300307</t>
   </si>
 </sst>
 </file>
@@ -114,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,147 +158,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,33 +480,41 @@
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -624,23 +526,35 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" customFormat="1">
-      <c r="A4" s="5" t="s">
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" customFormat="1">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -653,26 +567,36 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" customFormat="1">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -680,12 +604,20 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -697,10 +629,12 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -712,10 +646,12 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -727,10 +663,12 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -738,24 +676,34 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>